<commit_message>
Additional transactions added to overflow page one
</commit_message>
<xml_diff>
--- a/Transactions_File.xlsx
+++ b/Transactions_File.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHub\New folder\Invoices\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHub\Invoices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7214657-A14D-40B5-9BEE-1B641037681B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD44B7DC-2D27-4E94-8E36-37D71DDB653E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -358,10 +358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,6 +558,142 @@
         <v>41</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>45254</v>
+      </c>
+      <c r="E12">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13" s="1">
+        <v>45254</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>45254</v>
+      </c>
+      <c r="E14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>45254</v>
+      </c>
+      <c r="E15">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1">
+        <v>45254</v>
+      </c>
+      <c r="E16">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17" s="1">
+        <v>45254</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>45254</v>
+      </c>
+      <c r="E18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>45254</v>
+      </c>
+      <c r="E19">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>